<commit_message>
fix min_pack in master barang
</commit_message>
<xml_diff>
--- a/public/excel/import-barang.xlsx
+++ b/public/excel/import-barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37ABA1AE-328A-408B-9835-9ACCC636D894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C672BEB-893B-40D7-8F01-619D3EB524AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
+    <workbookView xWindow="0" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nama Suplier</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Import Data Barang</t>
+  </si>
+  <si>
+    <t>Min Qty (Jumlah renteng dalam satu dus)</t>
   </si>
 </sst>
 </file>
@@ -443,9 +446,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011259D-7C4D-4D1A-ACAD-A76A901F2A1A}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -456,14 +461,15 @@
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -493,6 +499,9 @@
       </c>
       <c r="J4" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create component penjualans invoice and change sturktur table of barang
</commit_message>
<xml_diff>
--- a/public/excel/import-barang.xlsx
+++ b/public/excel/import-barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C672BEB-893B-40D7-8F01-619D3EB524AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58EC74-683C-403E-9FE9-3DAE78766FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nama Suplier</t>
   </si>
@@ -45,22 +45,10 @@
     <t>Nama Barang</t>
   </si>
   <si>
-    <t>Kredit Dus</t>
-  </si>
-  <si>
-    <t>Kredit Pack</t>
-  </si>
-  <si>
-    <t>Kredit Pcs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cash Dus </t>
   </si>
   <si>
     <t>Cash Pack</t>
-  </si>
-  <si>
-    <t>Cash Pcs</t>
   </si>
   <si>
     <t>Diskon</t>
@@ -446,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011259D-7C4D-4D1A-ACAD-A76A901F2A1A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,19 +445,16 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,19 +474,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merubah struktur data barang
</commit_message>
<xml_diff>
--- a/public/excel/import-barang.xlsx
+++ b/public/excel/import-barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58EC74-683C-403E-9FE9-3DAE78766FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4628F705-1605-48D4-9B71-2FC884344509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
+    <workbookView xWindow="885" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nama Suplier</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Min Qty (Jumlah renteng dalam satu dus)</t>
+  </si>
+  <si>
+    <t>Harga Beli Dus</t>
+  </si>
+  <si>
+    <t>Harga Beli Pack</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011259D-7C4D-4D1A-ACAD-A76A901F2A1A}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,15 +452,19 @@
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,9 +481,15 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ubha struktur master barang menambahkan field kredit dus dan pack
</commit_message>
<xml_diff>
--- a/public/excel/import-barang.xlsx
+++ b/public/excel/import-barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4628F705-1605-48D4-9B71-2FC884344509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68A5811-A638-426F-8D96-D58413DC8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nama Suplier</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Harga Beli Pack</t>
+  </si>
+  <si>
+    <t>Kredit Dus</t>
+  </si>
+  <si>
+    <t>Kredit Pack</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011259D-7C4D-4D1A-ACAD-A76A901F2A1A}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,16 +461,17 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,9 +494,15 @@
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
menambahkab mengurutkan nota berdasarkan jenis barang
</commit_message>
<xml_diff>
--- a/public/excel/import-barang.xlsx
+++ b/public/excel/import-barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\taremakmur\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68A5811-A638-426F-8D96-D58413DC8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F83EBAE-8367-467E-A163-19C1C7F98224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{491C5DD8-1C3E-4BFB-8A29-27541AA19B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nama Suplier</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Kredit Pack</t>
+  </si>
+  <si>
+    <t>Jenis Barang</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011259D-7C4D-4D1A-ACAD-A76A901F2A1A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,14 +469,15 @@
     <col min="8" max="9" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,6 +510,9 @@
       </c>
       <c r="K4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>